<commit_message>
Changed connections excel sheet
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7863ff1081637df6/Bureaublad/Sem6_Project/universal_connector_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FAA0A33-4F46-4E61-8AB5-4F8E71E1883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{2FAA0A33-4F46-4E61-8AB5-4F8E71E1883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CFF16C-AD55-4BA3-952A-42E1C06EC36E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C545162B-9807-4C86-9800-C476C414EC09}"/>
   </bookViews>
@@ -1434,9 +1434,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6C3837-B0FE-41B2-B168-056701E2D3A6}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>